<commit_message>
BLSA and BGISA debugging
Add dark mode and tooltip improvements
</commit_message>
<xml_diff>
--- a/laws_import.xlsx
+++ b/laws_import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22adfb32f6bb0bcc/Desktop/ip-privacy-tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93795A79-341E-4269-AB0D-D13122AA9651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{93795A79-341E-4269-AB0D-D13122AA9651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2298F75-FC17-4C6F-BFC2-38C2497F3C54}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-250" yWindow="70" windowWidth="9710" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="140">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -433,10 +433,13 @@
     <t>Strong</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
     <t>Weak</t>
+  </si>
+  <si>
+    <t>Weak (currently)</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
   </si>
 </sst>
 </file>
@@ -806,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -921,7 +924,7 @@
         <v>132</v>
       </c>
       <c r="F5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G5">
         <v>5</v>
@@ -1151,7 +1154,7 @@
         <v>130</v>
       </c>
       <c r="F15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G15">
         <v>8</v>
@@ -1174,7 +1177,7 @@
         <v>131</v>
       </c>
       <c r="F16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G16">
         <v>8</v>
@@ -1197,7 +1200,7 @@
         <v>131</v>
       </c>
       <c r="F17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G17">
         <v>8</v>
@@ -1220,7 +1223,7 @@
         <v>133</v>
       </c>
       <c r="F18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G18">
         <v>8</v>
@@ -1243,7 +1246,7 @@
         <v>133</v>
       </c>
       <c r="F19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G19">
         <v>8</v>
@@ -1266,7 +1269,7 @@
         <v>133</v>
       </c>
       <c r="F20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G20">
         <v>8</v>
@@ -1289,7 +1292,7 @@
         <v>133</v>
       </c>
       <c r="F21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G21">
         <v>8</v>
@@ -1312,7 +1315,7 @@
         <v>131</v>
       </c>
       <c r="F22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G22">
         <v>8</v>
@@ -1335,7 +1338,7 @@
         <v>131</v>
       </c>
       <c r="F23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G23">
         <v>8</v>
@@ -1358,7 +1361,7 @@
         <v>134</v>
       </c>
       <c r="F24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G24">
         <v>8</v>
@@ -1381,7 +1384,7 @@
         <v>133</v>
       </c>
       <c r="F25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G25">
         <v>5</v>
@@ -1404,7 +1407,7 @@
         <v>131</v>
       </c>
       <c r="F26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G26">
         <v>5</v>
@@ -1427,7 +1430,7 @@
         <v>131</v>
       </c>
       <c r="F27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G27">
         <v>5</v>
@@ -1450,7 +1453,7 @@
         <v>133</v>
       </c>
       <c r="F28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G28">
         <v>5</v>
@@ -1473,7 +1476,7 @@
         <v>131</v>
       </c>
       <c r="F29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G29">
         <v>5</v>
@@ -1496,7 +1499,7 @@
         <v>134</v>
       </c>
       <c r="F30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G30">
         <v>5</v>
@@ -1519,7 +1522,7 @@
         <v>132</v>
       </c>
       <c r="F31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G31">
         <v>5</v>
@@ -1542,7 +1545,7 @@
         <v>131</v>
       </c>
       <c r="F32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G32">
         <v>5</v>
@@ -1565,7 +1568,7 @@
         <v>131</v>
       </c>
       <c r="F33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G33">
         <v>5</v>
@@ -1588,7 +1591,7 @@
         <v>131</v>
       </c>
       <c r="F34" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G34">
         <v>5</v>
@@ -1611,7 +1614,7 @@
         <v>133</v>
       </c>
       <c r="F35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G35">
         <v>5</v>
@@ -1634,7 +1637,7 @@
         <v>135</v>
       </c>
       <c r="F36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G36">
         <v>5</v>
@@ -1657,7 +1660,7 @@
         <v>133</v>
       </c>
       <c r="F37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G37">
         <v>5</v>
@@ -1680,7 +1683,7 @@
         <v>133</v>
       </c>
       <c r="F38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G38">
         <v>5</v>
@@ -1726,7 +1729,7 @@
         <v>133</v>
       </c>
       <c r="F40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G40">
         <v>5</v>
@@ -1749,7 +1752,7 @@
         <v>131</v>
       </c>
       <c r="F41" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G41">
         <v>5</v>
@@ -1772,7 +1775,7 @@
         <v>131</v>
       </c>
       <c r="F42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G42">
         <v>5</v>
@@ -1795,7 +1798,7 @@
         <v>131</v>
       </c>
       <c r="F43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G43">
         <v>5</v>
@@ -1818,7 +1821,7 @@
         <v>131</v>
       </c>
       <c r="F44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G44">
         <v>5</v>
@@ -1841,7 +1844,7 @@
         <v>131</v>
       </c>
       <c r="F45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G45">
         <v>5</v>
@@ -1864,7 +1867,7 @@
         <v>135</v>
       </c>
       <c r="F46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G46">
         <v>5</v>
@@ -1887,7 +1890,7 @@
         <v>133</v>
       </c>
       <c r="F47" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G47">
         <v>5</v>
@@ -1910,7 +1913,7 @@
         <v>133</v>
       </c>
       <c r="F48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G48">
         <v>5</v>
@@ -1933,7 +1936,7 @@
         <v>130</v>
       </c>
       <c r="F49" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G49">
         <v>5</v>
@@ -1956,7 +1959,7 @@
         <v>135</v>
       </c>
       <c r="F50" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G50">
         <v>5</v>
@@ -1979,7 +1982,7 @@
         <v>131</v>
       </c>
       <c r="F51" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G51">
         <v>5</v>
@@ -2002,7 +2005,7 @@
         <v>133</v>
       </c>
       <c r="F52" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G52">
         <v>5</v>

</xml_diff>

<commit_message>
Fixed symbol conversion issues pointed out by Zainab
cleaned up dataset
</commit_message>
<xml_diff>
--- a/laws_import.xlsx
+++ b/laws_import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22adfb32f6bb0bcc/Desktop/ip-privacy-tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{93795A79-341E-4269-AB0D-D13122AA9651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2298F75-FC17-4C6F-BFC2-38C2497F3C54}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{93795A79-341E-4269-AB0D-D13122AA9651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{237B39AE-8654-4F5D-AC43-9AD17C83B1DD}"/>
   <bookViews>
-    <workbookView xWindow="-250" yWindow="70" windowWidth="9710" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,24 +67,6 @@
     <t>Copyright Act, 17 U.S.C. (1976)</t>
   </si>
   <si>
-    <t>DMCA, 17 U.S.C. Â§ 512</t>
-  </si>
-  <si>
-    <t>Hatch-Waxman Act, 21 U.S.C. Â§ 355</t>
-  </si>
-  <si>
-    <t>Patent Term Restoration, 35 U.S.C. Â§ 154</t>
-  </si>
-  <si>
-    <t>Paragraph IV Certifications, 21 U.S.C. Â§ 355(j)(2)(A)(vii)</t>
-  </si>
-  <si>
-    <t>Design Patents, 35 U.S.C. Â§ 171</t>
-  </si>
-  <si>
-    <t>Defend Trade Secrets Act, 18 U.S.C. Â§ 1836</t>
-  </si>
-  <si>
     <t>GLBA</t>
   </si>
   <si>
@@ -109,9 +91,6 @@
     <t>Trademarks Act</t>
   </si>
   <si>
-    <t>Criminal Code, ss. 406â€“409</t>
-  </si>
-  <si>
     <t>Patented Medicines Regulations</t>
   </si>
   <si>
@@ -256,9 +235,6 @@
     <t>Provides protection for inventions including pharmaceuticals and biotech.</t>
   </si>
   <si>
-    <t>Protects creatorsâ€™ rights in literary, musical, and artistic works.</t>
-  </si>
-  <si>
     <t>Protects brand identifiers like logos and names.</t>
   </si>
   <si>
@@ -440,6 +416,30 @@
   </si>
   <si>
     <t>Not Applicable</t>
+  </si>
+  <si>
+    <t>Protects creators'™ rights in literary, musical, and artistic works.</t>
+  </si>
+  <si>
+    <t>Criminal Code, ss. 406 &amp; 409</t>
+  </si>
+  <si>
+    <t>DMCA, 17 U.S.C. § 512</t>
+  </si>
+  <si>
+    <t>Hatch-Waxman Act, 21 U.S.C. § 355</t>
+  </si>
+  <si>
+    <t>Patent Term Restoration, 35 U.S.C. § 154</t>
+  </si>
+  <si>
+    <t>Paragraph IV Certifications, 21 U.S.C. § 355(j)(2)(A)(vii)</t>
+  </si>
+  <si>
+    <t>Design Patents, 35 U.S.C. § 171</t>
+  </si>
+  <si>
+    <t>Defend Trade Secrets Act, 18 U.S.C. § 1836</t>
   </si>
 </sst>
 </file>
@@ -518,6 +518,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -809,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -846,16 +850,16 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G2">
         <v>4</v>
@@ -869,16 +873,16 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E3" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -889,19 +893,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>134</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E4" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F4" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -912,19 +916,19 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>135</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F5" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G5">
         <v>5</v>
@@ -935,19 +939,19 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E6" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F6" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G6">
         <v>4</v>
@@ -958,19 +962,19 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>137</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D7" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E7" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F7" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G7">
         <v>4</v>
@@ -981,19 +985,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>138</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E8" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F8" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G8">
         <v>4</v>
@@ -1004,19 +1008,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>139</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E9" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F9" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G9">
         <v>4</v>
@@ -1027,19 +1031,19 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D10" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="E10" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F10" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G10">
         <v>4</v>
@@ -1050,19 +1054,19 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E11" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F11" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G11">
         <v>4</v>
@@ -1073,19 +1077,19 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E12" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F12" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G12">
         <v>4</v>
@@ -1096,19 +1100,19 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E13" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F13" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G13">
         <v>4</v>
@@ -1119,19 +1123,19 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D14" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E14" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F14" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G14">
         <v>4</v>
@@ -1142,19 +1146,19 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E15" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F15" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G15">
         <v>8</v>
@@ -1165,19 +1169,19 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="D16" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E16" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F16" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G16">
         <v>8</v>
@@ -1188,19 +1192,19 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E17" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F17" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G17">
         <v>8</v>
@@ -1211,19 +1215,19 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>133</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D18" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E18" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F18" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G18">
         <v>8</v>
@@ -1234,19 +1238,19 @@
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D19" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E19" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F19" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G19">
         <v>8</v>
@@ -1257,19 +1261,19 @@
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D20" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" t="s">
         <v>125</v>
       </c>
-      <c r="E20" t="s">
-        <v>133</v>
-      </c>
       <c r="F20" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G20">
         <v>8</v>
@@ -1280,19 +1284,19 @@
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D21" t="s">
+        <v>117</v>
+      </c>
+      <c r="E21" t="s">
         <v>125</v>
       </c>
-      <c r="E21" t="s">
-        <v>133</v>
-      </c>
       <c r="F21" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G21">
         <v>8</v>
@@ -1303,19 +1307,19 @@
         <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D22" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E22" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F22" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G22">
         <v>8</v>
@@ -1326,19 +1330,19 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D23" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E23" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F23" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G23">
         <v>8</v>
@@ -1349,19 +1353,19 @@
         <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D24" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" t="s">
         <v>126</v>
       </c>
-      <c r="E24" t="s">
-        <v>134</v>
-      </c>
       <c r="F24" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G24">
         <v>8</v>
@@ -1372,19 +1376,19 @@
         <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D25" t="s">
+        <v>117</v>
+      </c>
+      <c r="E25" t="s">
         <v>125</v>
       </c>
-      <c r="E25" t="s">
-        <v>133</v>
-      </c>
       <c r="F25" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G25">
         <v>5</v>
@@ -1395,19 +1399,19 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D26" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E26" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F26" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G26">
         <v>5</v>
@@ -1418,19 +1422,19 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D27" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E27" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F27" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G27">
         <v>5</v>
@@ -1441,19 +1445,19 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D28" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="E28" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F28" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G28">
         <v>5</v>
@@ -1464,19 +1468,19 @@
         <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D29" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E29" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F29" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G29">
         <v>5</v>
@@ -1487,19 +1491,19 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D30" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E30" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="F30" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G30">
         <v>5</v>
@@ -1510,19 +1514,19 @@
         <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D31" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E31" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F31" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G31">
         <v>5</v>
@@ -1533,19 +1537,19 @@
         <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D32" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E32" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F32" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G32">
         <v>5</v>
@@ -1556,19 +1560,19 @@
         <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D33" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E33" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F33" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G33">
         <v>5</v>
@@ -1579,19 +1583,19 @@
         <v>10</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D34" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E34" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F34" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G34">
         <v>5</v>
@@ -1602,19 +1606,19 @@
         <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D35" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E35" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F35" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G35">
         <v>5</v>
@@ -1625,19 +1629,19 @@
         <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D36" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="E36" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F36" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G36">
         <v>5</v>
@@ -1648,19 +1652,19 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D37" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="E37" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F37" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G37">
         <v>5</v>
@@ -1671,19 +1675,19 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D38" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="E38" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F38" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G38">
         <v>5</v>
@@ -1694,19 +1698,19 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C39" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D39" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E39" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F39" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G39">
         <v>5</v>
@@ -1717,19 +1721,19 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C40" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D40" t="s">
+        <v>117</v>
+      </c>
+      <c r="E40" t="s">
         <v>125</v>
       </c>
-      <c r="E40" t="s">
-        <v>133</v>
-      </c>
       <c r="F40" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G40">
         <v>5</v>
@@ -1740,19 +1744,19 @@
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C41" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D41" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E41" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F41" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G41">
         <v>5</v>
@@ -1763,19 +1767,19 @@
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C42" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D42" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E42" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F42" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G42">
         <v>5</v>
@@ -1786,19 +1790,19 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C43" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D43" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E43" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F43" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G43">
         <v>5</v>
@@ -1809,19 +1813,19 @@
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C44" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D44" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E44" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F44" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G44">
         <v>5</v>
@@ -1832,19 +1836,19 @@
         <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C45" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D45" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E45" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F45" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G45">
         <v>5</v>
@@ -1855,19 +1859,19 @@
         <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C46" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46" t="s">
         <v>108</v>
       </c>
-      <c r="D46" t="s">
-        <v>116</v>
-      </c>
       <c r="E46" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F46" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G46">
         <v>5</v>
@@ -1878,19 +1882,19 @@
         <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C47" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D47" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="E47" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F47" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="G47">
         <v>5</v>
@@ -1901,19 +1905,19 @@
         <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C48" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D48" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="E48" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F48" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G48">
         <v>5</v>
@@ -1924,19 +1928,19 @@
         <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C49" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D49" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E49" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F49" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="G49">
         <v>5</v>
@@ -1947,19 +1951,19 @@
         <v>12</v>
       </c>
       <c r="B50" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C50" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D50" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E50" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F50" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="G50">
         <v>5</v>
@@ -1970,19 +1974,19 @@
         <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C51" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D51" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E51" t="s">
+        <v>123</v>
+      </c>
+      <c r="F51" t="s">
         <v>131</v>
-      </c>
-      <c r="F51" t="s">
-        <v>139</v>
       </c>
       <c r="G51">
         <v>5</v>
@@ -1993,19 +1997,19 @@
         <v>12</v>
       </c>
       <c r="B52" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C52" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D52" t="s">
+        <v>117</v>
+      </c>
+      <c r="E52" t="s">
         <v>125</v>
       </c>
-      <c r="E52" t="s">
-        <v>133</v>
-      </c>
       <c r="F52" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="G52">
         <v>5</v>

</xml_diff>